<commit_message>
ajustes de reportes en backend
</commit_message>
<xml_diff>
--- a/docs/formatos/reporteGeneral.xlsx
+++ b/docs/formatos/reporteGeneral.xlsx
@@ -16,37 +16,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
-    <t>Usuarios registrados</t>
-  </si>
-  <si>
-    <t>Usuarios activos</t>
-  </si>
-  <si>
-    <t>Usuarios inactivos</t>
-  </si>
-  <si>
-    <t>Programas</t>
-  </si>
-  <si>
     <t>Fecha inicio</t>
   </si>
   <si>
     <t>Fecha fin</t>
   </si>
   <si>
-    <t>Usuarios no iniciados</t>
-  </si>
-  <si>
-    <t>Usuarios cursando</t>
-  </si>
-  <si>
-    <t>Usuarios finalizado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listado de participantes. </t>
   </si>
   <si>
     <t xml:space="preserve">Empresa: Link Gerencial. </t>
+  </si>
+  <si>
+    <t>Programa</t>
+  </si>
+  <si>
+    <t>Participantes registrados</t>
+  </si>
+  <si>
+    <t>Participantes activos</t>
+  </si>
+  <si>
+    <t>Participantes inactivos</t>
+  </si>
+  <si>
+    <t>Participantes no iniciados</t>
+  </si>
+  <si>
+    <t>Participantes cursando</t>
+  </si>
+  <si>
+    <t>Participantes finalizado</t>
   </si>
 </sst>
 </file>
@@ -101,12 +101,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,175 +410,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
ajuste en reporte de avance
</commit_message>
<xml_diff>
--- a/docs/formatos/reporteGeneral.xlsx
+++ b/docs/formatos/reporteGeneral.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC0EAF0-EB3F-428A-BC9D-B342646C484F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participantes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -59,16 +60,16 @@
     <t>Participantes cursando</t>
   </si>
   <si>
-    <t>Participantes finalizado</t>
-  </si>
-  <si>
     <t>Participantes sin acceso</t>
+  </si>
+  <si>
+    <t>Participantes aprobado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,9 +129,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +144,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -427,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,162 +449,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>